<commit_message>
added coefficients for thermistors andsome minor changes to gui
</commit_message>
<xml_diff>
--- a/thermode/Thermistor Heizmatte 24V 150W.xlsx
+++ b/thermode/Thermistor Heizmatte 24V 150W.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\git\PythonCanSteering\thermode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE213FF-DC75-4ACF-B4A2-B762BFE65F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0531E1-FD94-4AA9-B1E7-86AC0245E2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C380DCA7-C0C2-43C0-A75E-3FD818F4CEDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C380DCA7-C0C2-43C0-A75E-3FD818F4CEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Bett" sheetId="1" r:id="rId1"/>
     <sheet name="Thermode" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>°C</t>
   </si>
@@ -110,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,17 +117,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2012,232 +2022,232 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>186.99087994817421</c:v>
+                  <c:v>159.47977269093968</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>172.8</c:v>
+                  <c:v>148.1050804777089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>172.05641786320336</c:v>
+                  <c:v>147.50570353078228</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>164.23786522102694</c:v>
+                  <c:v>141.18449333155831</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>151.01830423855108</c:v>
+                  <c:v>130.42386353041098</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>148.78564218623234</c:v>
+                  <c:v>128.59830771016328</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>148.65092648344472</c:v>
+                  <c:v>128.48808615562757</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>146.31495877500697</c:v>
+                  <c:v>126.57561055930881</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>140.56034010211749</c:v>
+                  <c:v>121.85475386590798</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>136.72221142891533</c:v>
+                  <c:v>118.69914506757601</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>132.53729898464547</c:v>
+                  <c:v>115.25267703011616</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>128.55775609780625</c:v>
+                  <c:v>111.9703182551707</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>123.2926741726493</c:v>
+                  <c:v>107.62104802571662</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>118.60339668651915</c:v>
+                  <c:v>103.74207716485631</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>116.80000000000001</c:v>
+                  <c:v>102.24917766463869</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>112.30469570509695</c:v>
+                  <c:v>98.525610180527281</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104.99368363887413</c:v>
+                  <c:v>92.464848893193619</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>99.196626446727976</c:v>
+                  <c:v>87.657134742515723</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>94.412126585594763</c:v>
+                  <c:v>83.689438768565253</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>90.350096540715356</c:v>
+                  <c:v>80.322024672521934</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>86.828162509337972</c:v>
+                  <c:v>77.403822465220742</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>83.724476152988814</c:v>
+                  <c:v>74.833724157650806</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>80.953746184653539</c:v>
+                  <c:v>72.540863647018739</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>78.454029585516935</c:v>
+                  <c:v>70.473722596398204</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>76.178974607678583</c:v>
+                  <c:v>68.593720155413337</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>74.093026786752773</c:v>
+                  <c:v>66.871244878501045</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>72.168339183640228</c:v>
+                  <c:v>65.283093838918887</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>70.382709802743364</c:v>
+                  <c:v>63.810761173693152</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>68.718162960782081</c:v>
+                  <c:v>62.439259834308814</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>67.159948144430189</c:v>
+                  <c:v>61.156289410257727</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>65.695817503938486</c:v>
+                  <c:v>59.951635145991702</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>64.315494081176951</c:v>
+                  <c:v>58.816725348239231</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>63.010273546488008</c:v>
+                  <c:v>57.744299742839246</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>61.772721257400519</c:v>
+                  <c:v>56.728157097211749</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>60.596438590419154</c:v>
+                  <c:v>55.762960479709136</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>59.475880423598937</c:v>
+                  <c:v>54.844085098707637</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>58.406210936396235</c:v>
+                  <c:v>53.967498052288249</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>57.383188491301723</c:v>
+                  <c:v>53.129662306539444</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>56.403072853061701</c:v>
+                  <c:v>52.327459290100307</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>55.462549754223971</c:v>
+                  <c:v>51.558125949561088</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>54.558669067420567</c:v>
+                  <c:v>50.819203151212207</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>53.68879375071873</c:v>
+                  <c:v>50.108493068315852</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>52.04182870459482</c:v>
+                  <c:v>48.764019442707479</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>51.260681575880767</c:v>
+                  <c:v>48.126875664621593</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>49.774305447067604</c:v>
+                  <c:v>46.915484234866312</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>48.379251159693354</c:v>
+                  <c:v>45.779709506881716</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>47.712723712716922</c:v>
+                  <c:v>45.237476535796759</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>47.065343195370417</c:v>
+                  <c:v>44.711082059290391</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>46.436082826999439</c:v>
+                  <c:v>44.199671891808862</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>45.823995062909262</c:v>
+                  <c:v>43.702457925832618</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>45.228203708485296</c:v>
+                  <c:v>43.218711548559099</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>44.647896985910393</c:v>
+                  <c:v>42.7477578541139</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>44.082321419089794</c:v>
+                  <c:v>42.288970539065588</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>43.530776423956581</c:v>
+                  <c:v>41.84176738702007</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42.992609509030672</c:v>
+                  <c:v>41.405606262849744</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42.467212005709996</c:v>
+                  <c:v>40.979981549303602</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>41.954015259869834</c:v>
+                  <c:v>40.56442096885354</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>41.452487226420203</c:v>
+                  <c:v>40.158482742037222</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>40.96212941687952</c:v>
+                  <c:v>39.761753040585575</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>36.582471564988907</c:v>
+                  <c:v>36.225890653631382</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>35.803360723465346</c:v>
+                  <c:v>35.598350015489984</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>35.424109978475258</c:v>
+                  <c:v>35.293044230362625</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>35.051424162508397</c:v>
+                  <c:v>34.993129114579233</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>34.324898276264378</c:v>
+                  <c:v>34.408768285365454</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>32.941824566393052</c:v>
+                  <c:v>33.297453281888124</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>30.718444032680054</c:v>
+                  <c:v>31.514086930318797</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>30.123786223340858</c:v>
+                  <c:v>31.03778333890574</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>29.832620233068099</c:v>
+                  <c:v>30.80467230007622</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>29.545419310446164</c:v>
+                  <c:v>30.574803341886877</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>29.262080943681383</c:v>
+                  <c:v>30.34809191082627</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>28.982506490047115</c:v>
+                  <c:v>30.124456659885993</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>28.706600985044645</c:v>
+                  <c:v>29.903819289938951</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>28.326323599146519</c:v>
+                  <c:v>29.599820378379434</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>28.165434289197947</c:v>
+                  <c:v>29.471239350937196</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>28.005770499740834</c:v>
+                  <c:v>29.343659012487819</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>27.900000000000034</c:v>
+                  <c:v>29.259154126222029</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3624,16 +3634,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3960,8 +3970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748DA434-C63D-43E5-8424-EEB26822DEA9}">
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="H50" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4706,16 +4716,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC81097-07E4-4189-A5AA-3B0771035039}">
-  <dimension ref="A1:Y77"/>
+  <dimension ref="A1:Y90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="96" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="11.42578125" style="1"/>
     <col min="6" max="6" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
+    <col min="13" max="23" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -4736,21 +4748,21 @@
       </c>
       <c r="F1" s="2">
         <f>F7</f>
-        <v>2.2863002829186085E-3</v>
+        <v>2.4135089308139767E-3</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
       </c>
       <c r="L1">
-        <f>LN(A3)</f>
-        <v>-0.19845093872383832</v>
+        <f>LN(A84)</f>
+        <v>1.8946168546677629</v>
       </c>
       <c r="X1" t="s">
         <v>10</v>
       </c>
       <c r="Y1">
-        <f>1/(B3+273.15)</f>
-        <v>2.2424038569346339E-3</v>
+        <f>1/(B84+273.15)</f>
+        <v>2.7921262041044259E-3</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -4761,33 +4773,33 @@
         <v>186.6</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C77" si="0">1/($F$1+$F$2*LN(A2)+$F$3*LN(A2)^3)-273.15</f>
-        <v>186.99087994817421</v>
+        <f t="shared" ref="C2:C78" si="0">1/($F$1+$F$2*LN(A2)+$F$3*LN(A2)^3)-273.15</f>
+        <v>159.47977269093968</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="3">
         <f>F6</f>
-        <v>2.2117428114341894E-4</v>
+        <v>1.9979867066601524E-4</v>
       </c>
       <c r="G2">
         <f>(Y2-Y1)/(L2-L1)</f>
-        <v>2.2190214606844055E-4</v>
+        <v>1.9984352367242241E-4</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
       </c>
       <c r="L2">
-        <f>LN(A16)</f>
-        <v>1.2527629684953681</v>
+        <f>LN(A86)</f>
+        <v>-2.1119647333853959</v>
       </c>
       <c r="X2" t="s">
         <v>11</v>
       </c>
       <c r="Y2">
-        <f>1/(B16+273.15)</f>
-        <v>2.5644313373509426E-3</v>
+        <f>1/(B86+273.15)</f>
+        <v>1.9914368216668327E-3</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -4799,7 +4811,7 @@
       </c>
       <c r="C3" s="1">
         <f t="shared" si="0"/>
-        <v>172.8</v>
+        <v>148.1050804777089</v>
       </c>
       <c r="D3">
         <v>7.78</v>
@@ -4809,25 +4821,25 @@
       </c>
       <c r="F3" s="3">
         <f>F5</f>
-        <v>5.3512167374125338E-7</v>
+        <v>1.1078634885733181E-8</v>
       </c>
       <c r="G3">
         <f>(Y3-Y1)/(L3-L1)</f>
-        <v>2.3139374292805416E-4</v>
+        <v>2.0016819399749572E-4</v>
       </c>
       <c r="K3" t="s">
         <v>9</v>
       </c>
       <c r="L3">
-        <f>LN(A77)</f>
-        <v>4.4659081186545837</v>
+        <f>LN(A88)</f>
+        <v>4.5900565481780431</v>
       </c>
       <c r="X3" t="s">
         <v>12</v>
       </c>
       <c r="Y3">
-        <f>1/(B77+273.15)</f>
-        <v>3.3217073575817976E-3</v>
+        <f>1/(B88+273.15)</f>
+        <v>3.331667499583542E-3</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -4839,7 +4851,7 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>172.05641786320336</v>
+        <v>147.50570353078228</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -4851,14 +4863,14 @@
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>164.23786522102694</v>
+        <v>141.18449333155831</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="3">
         <f>(G3-G2)/(L3-L2)/(L1+L2+L3)</f>
-        <v>5.3512167374125338E-7</v>
+        <v>1.1078634885733181E-8</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -4870,7 +4882,7 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>151.01830423855108</v>
+        <v>130.42386353041098</v>
       </c>
       <c r="D6">
         <v>7.71</v>
@@ -4880,7 +4892,7 @@
       </c>
       <c r="F6" s="3">
         <f>G2-F5*(L1*L1+L1*L2+L2*L2)</f>
-        <v>2.2117428114341894E-4</v>
+        <v>1.9979867066601524E-4</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -4892,7 +4904,7 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>148.78564218623234</v>
+        <v>128.59830771016328</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -4902,7 +4914,7 @@
       </c>
       <c r="F7" s="3">
         <f>Y1-(F6+L1*L1*F5)*L1</f>
-        <v>2.2863002829186085E-3</v>
+        <v>2.4135089308139767E-3</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -4914,7 +4926,7 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>148.65092648344472</v>
+        <v>128.48808615562757</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -4929,7 +4941,7 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>146.31495877500697</v>
+        <v>126.57561055930881</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -4941,7 +4953,7 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>140.56034010211749</v>
+        <v>121.85475386590798</v>
       </c>
       <c r="D10">
         <v>7.01</v>
@@ -4956,7 +4968,7 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>136.72221142891533</v>
+        <v>118.69914506757601</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -4971,7 +4983,7 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>132.53729898464547</v>
+        <v>115.25267703011616</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -4983,7 +4995,7 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>128.55775609780625</v>
+        <v>111.9703182551707</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -4998,7 +5010,7 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>123.2926741726493</v>
+        <v>107.62104802571662</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -5013,7 +5025,7 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>118.60339668651915</v>
+        <v>103.74207716485631</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -5025,7 +5037,7 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>116.80000000000001</v>
+        <v>102.24917766463869</v>
       </c>
       <c r="D16">
         <v>5.99</v>
@@ -5040,7 +5052,7 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
-        <v>112.30469570509695</v>
+        <v>98.525610180527281</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5052,7 +5064,7 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
-        <v>104.99368363887413</v>
+        <v>92.464848893193619</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5064,7 +5076,7 @@
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
-        <v>99.196626446727976</v>
+        <v>87.657134742515723</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5073,7 +5085,7 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
-        <v>94.412126585594763</v>
+        <v>83.689438768565253</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5085,7 +5097,7 @@
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
-        <v>90.350096540715356</v>
+        <v>80.322024672521934</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -5100,7 +5112,7 @@
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
-        <v>86.828162509337972</v>
+        <v>77.403822465220742</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5112,7 +5124,7 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
-        <v>83.724476152988814</v>
+        <v>74.833724157650806</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5124,7 +5136,7 @@
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
-        <v>80.953746184653539</v>
+        <v>72.540863647018739</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5136,7 +5148,7 @@
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
-        <v>78.454029585516935</v>
+        <v>70.473722596398204</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5148,7 +5160,7 @@
       </c>
       <c r="C26" s="1">
         <f t="shared" si="0"/>
-        <v>76.178974607678583</v>
+        <v>68.593720155413337</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5160,7 +5172,7 @@
       </c>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
-        <v>74.093026786752773</v>
+        <v>66.871244878501045</v>
       </c>
       <c r="D27">
         <v>3.97</v>
@@ -5175,7 +5187,7 @@
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
-        <v>72.168339183640228</v>
+        <v>65.283093838918887</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5187,7 +5199,7 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" si="0"/>
-        <v>70.382709802743364</v>
+        <v>63.810761173693152</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5199,7 +5211,7 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
-        <v>68.718162960782081</v>
+        <v>62.439259834308814</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5211,7 +5223,7 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
-        <v>67.159948144430189</v>
+        <v>61.156289410257727</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5223,7 +5235,7 @@
       </c>
       <c r="C32" s="1">
         <f t="shared" si="0"/>
-        <v>65.695817503938486</v>
+        <v>59.951635145991702</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -5235,7 +5247,7 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" si="0"/>
-        <v>64.315494081176951</v>
+        <v>58.816725348239231</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -5247,7 +5259,7 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" si="0"/>
-        <v>63.010273546488008</v>
+        <v>57.744299742839246</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -5259,7 +5271,7 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" si="0"/>
-        <v>61.772721257400519</v>
+        <v>56.728157097211749</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -5271,7 +5283,7 @@
       </c>
       <c r="C36" s="1">
         <f t="shared" si="0"/>
-        <v>60.596438590419154</v>
+        <v>55.762960479709136</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -5283,7 +5295,7 @@
       </c>
       <c r="C37" s="1">
         <f t="shared" si="0"/>
-        <v>59.475880423598937</v>
+        <v>54.844085098707637</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -5295,7 +5307,7 @@
       </c>
       <c r="C38" s="1">
         <f t="shared" si="0"/>
-        <v>58.406210936396235</v>
+        <v>53.967498052288249</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -5307,7 +5319,7 @@
       </c>
       <c r="C39" s="1">
         <f t="shared" si="0"/>
-        <v>57.383188491301723</v>
+        <v>53.129662306539444</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -5319,7 +5331,7 @@
       </c>
       <c r="C40" s="1">
         <f t="shared" si="0"/>
-        <v>56.403072853061701</v>
+        <v>52.327459290100307</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -5331,7 +5343,7 @@
       </c>
       <c r="C41" s="1">
         <f t="shared" si="0"/>
-        <v>55.462549754223971</v>
+        <v>51.558125949561088</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -5343,7 +5355,7 @@
       </c>
       <c r="C42" s="1">
         <f t="shared" si="0"/>
-        <v>54.558669067420567</v>
+        <v>50.819203151212207</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -5355,7 +5367,7 @@
       </c>
       <c r="C43" s="1">
         <f t="shared" si="0"/>
-        <v>53.68879375071873</v>
+        <v>50.108493068315852</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -5367,7 +5379,7 @@
       </c>
       <c r="C44" s="1">
         <f t="shared" si="0"/>
-        <v>52.04182870459482</v>
+        <v>48.764019442707479</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -5379,7 +5391,7 @@
       </c>
       <c r="C45" s="1">
         <f t="shared" si="0"/>
-        <v>51.260681575880767</v>
+        <v>48.126875664621593</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -5391,7 +5403,7 @@
       </c>
       <c r="C46" s="1">
         <f t="shared" si="0"/>
-        <v>49.774305447067604</v>
+        <v>46.915484234866312</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -5403,7 +5415,7 @@
       </c>
       <c r="C47" s="1">
         <f t="shared" si="0"/>
-        <v>48.379251159693354</v>
+        <v>45.779709506881716</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -5415,7 +5427,7 @@
       </c>
       <c r="C48" s="1">
         <f t="shared" si="0"/>
-        <v>47.712723712716922</v>
+        <v>45.237476535796759</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -5427,7 +5439,7 @@
       </c>
       <c r="C49" s="1">
         <f t="shared" si="0"/>
-        <v>47.065343195370417</v>
+        <v>44.711082059290391</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -5439,7 +5451,7 @@
       </c>
       <c r="C50" s="1">
         <f t="shared" si="0"/>
-        <v>46.436082826999439</v>
+        <v>44.199671891808862</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -5451,7 +5463,7 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" si="0"/>
-        <v>45.823995062909262</v>
+        <v>43.702457925832618</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -5463,7 +5475,7 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" si="0"/>
-        <v>45.228203708485296</v>
+        <v>43.218711548559099</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -5475,7 +5487,7 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" si="0"/>
-        <v>44.647896985910393</v>
+        <v>42.7477578541139</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -5487,7 +5499,7 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" si="0"/>
-        <v>44.082321419089794</v>
+        <v>42.288970539065588</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -5499,7 +5511,7 @@
       </c>
       <c r="C55" s="1">
         <f t="shared" si="0"/>
-        <v>43.530776423956581</v>
+        <v>41.84176738702007</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -5511,7 +5523,7 @@
       </c>
       <c r="C56" s="1">
         <f t="shared" si="0"/>
-        <v>42.992609509030672</v>
+        <v>41.405606262849744</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -5523,7 +5535,7 @@
       </c>
       <c r="C57" s="1">
         <f t="shared" si="0"/>
-        <v>42.467212005709996</v>
+        <v>40.979981549303602</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -5535,7 +5547,7 @@
       </c>
       <c r="C58" s="1">
         <f t="shared" si="0"/>
-        <v>41.954015259869834</v>
+        <v>40.56442096885354</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -5547,7 +5559,7 @@
       </c>
       <c r="C59" s="1">
         <f t="shared" si="0"/>
-        <v>41.452487226420203</v>
+        <v>40.158482742037222</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -5559,7 +5571,7 @@
       </c>
       <c r="C60" s="1">
         <f t="shared" si="0"/>
-        <v>40.96212941687952</v>
+        <v>39.761753040585575</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -5571,7 +5583,7 @@
       </c>
       <c r="C61" s="1">
         <f t="shared" si="0"/>
-        <v>36.582471564988907</v>
+        <v>36.225890653631382</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -5583,7 +5595,7 @@
       </c>
       <c r="C62" s="1">
         <f t="shared" si="0"/>
-        <v>35.803360723465346</v>
+        <v>35.598350015489984</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -5595,7 +5607,7 @@
       </c>
       <c r="C63" s="1">
         <f t="shared" si="0"/>
-        <v>35.424109978475258</v>
+        <v>35.293044230362625</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -5607,7 +5619,7 @@
       </c>
       <c r="C64" s="1">
         <f t="shared" si="0"/>
-        <v>35.051424162508397</v>
+        <v>34.993129114579233</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -5619,7 +5631,7 @@
       </c>
       <c r="C65" s="1">
         <f t="shared" si="0"/>
-        <v>34.324898276264378</v>
+        <v>34.408768285365454</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -5631,7 +5643,7 @@
       </c>
       <c r="C66" s="1">
         <f t="shared" si="0"/>
-        <v>32.941824566393052</v>
+        <v>33.297453281888124</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -5643,7 +5655,7 @@
       </c>
       <c r="C67" s="1">
         <f t="shared" si="0"/>
-        <v>30.718444032680054</v>
+        <v>31.514086930318797</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -5655,7 +5667,7 @@
       </c>
       <c r="C68" s="1">
         <f t="shared" si="0"/>
-        <v>30.123786223340858</v>
+        <v>31.03778333890574</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -5667,7 +5679,7 @@
       </c>
       <c r="C69" s="1">
         <f t="shared" si="0"/>
-        <v>29.832620233068099</v>
+        <v>30.80467230007622</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -5679,7 +5691,7 @@
       </c>
       <c r="C70" s="1">
         <f t="shared" si="0"/>
-        <v>29.545419310446164</v>
+        <v>30.574803341886877</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -5691,7 +5703,7 @@
       </c>
       <c r="C71" s="1">
         <f t="shared" si="0"/>
-        <v>29.262080943681383</v>
+        <v>30.34809191082627</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -5703,7 +5715,7 @@
       </c>
       <c r="C72" s="1">
         <f t="shared" si="0"/>
-        <v>28.982506490047115</v>
+        <v>30.124456659885993</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -5715,7 +5727,7 @@
       </c>
       <c r="C73" s="1">
         <f t="shared" si="0"/>
-        <v>28.706600985044645</v>
+        <v>29.903819289938951</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -5727,7 +5739,7 @@
       </c>
       <c r="C74" s="1">
         <f t="shared" si="0"/>
-        <v>28.326323599146519</v>
+        <v>29.599820378379434</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -5739,7 +5751,7 @@
       </c>
       <c r="C75" s="1">
         <f t="shared" si="0"/>
-        <v>28.165434289197947</v>
+        <v>29.471239350937196</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -5751,26 +5763,192 @@
       </c>
       <c r="C76" s="1">
         <f t="shared" si="0"/>
-        <v>28.005770499740834</v>
+        <v>29.343659012487819</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77">
+      <c r="A77" s="4">
         <v>87</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="4">
         <v>27.9</v>
       </c>
-      <c r="C77" s="1">
-        <f t="shared" si="0"/>
-        <v>27.900000000000034</v>
+      <c r="C77" s="5">
+        <f t="shared" si="0"/>
+        <v>29.259154126222029</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
     </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>96.9</v>
+      </c>
+      <c r="B78">
+        <v>25.5</v>
+      </c>
+      <c r="C78" s="5">
+        <f t="shared" si="0"/>
+        <v>27.296105621683694</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
+        <v>0.161</v>
+      </c>
+      <c r="B79">
+        <v>250</v>
+      </c>
+      <c r="C79" s="5">
+        <f t="shared" ref="C79:C90" si="1">1/($F$1+$F$2*LN(A79)+$F$3*LN(A79)^3)-273.15</f>
+        <v>215.00278665789028</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80">
+        <v>97.3</v>
+      </c>
+      <c r="B80">
+        <v>24.3</v>
+      </c>
+      <c r="C80" s="5">
+        <f t="shared" si="1"/>
+        <v>27.221569063259835</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81">
+        <v>104.1</v>
+      </c>
+      <c r="B81">
+        <v>23.9</v>
+      </c>
+      <c r="C81" s="5">
+        <f t="shared" si="1"/>
+        <v>26.004472141586859</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82">
+        <v>5.44</v>
+      </c>
+      <c r="B82">
+        <v>100</v>
+      </c>
+      <c r="C82" s="5">
+        <f t="shared" si="1"/>
+        <v>90.225054746201636</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83">
+        <v>0.1363</v>
+      </c>
+      <c r="B83">
+        <v>260</v>
+      </c>
+      <c r="C83" s="5">
+        <f t="shared" si="1"/>
+        <v>223.06805345071075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84">
+        <v>6.65</v>
+      </c>
+      <c r="B84">
+        <v>85</v>
+      </c>
+      <c r="C84" s="5">
+        <f t="shared" si="1"/>
+        <v>85.000000000000057</v>
+      </c>
+      <c r="D84" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85">
+        <v>1.33</v>
+      </c>
+      <c r="B85">
+        <v>130</v>
+      </c>
+      <c r="C85" s="5">
+        <f t="shared" si="1"/>
+        <v>131.62839907292988</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86">
+        <v>0.121</v>
+      </c>
+      <c r="B86">
+        <v>229</v>
+      </c>
+      <c r="C86" s="5">
+        <f t="shared" si="1"/>
+        <v>229.00000000000011</v>
+      </c>
+      <c r="D86" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87">
+        <v>0.371</v>
+      </c>
+      <c r="B87">
+        <v>180</v>
+      </c>
+      <c r="C87" s="5">
+        <f t="shared" si="1"/>
+        <v>178.23837937923008</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88">
+        <v>98.5</v>
+      </c>
+      <c r="B88">
+        <v>27</v>
+      </c>
+      <c r="C88" s="5">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="D88" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89">
+        <v>0.747</v>
+      </c>
+      <c r="B89">
+        <v>150</v>
+      </c>
+      <c r="C89" s="1">
+        <f t="shared" si="1"/>
+        <v>151.43709787071168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="B90">
+        <v>170</v>
+      </c>
+      <c r="C90" s="1">
+        <f t="shared" si="1"/>
+        <v>179.69537543185322</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>